<commit_message>
Proposed Plan 2 sheet updated
</commit_message>
<xml_diff>
--- a/Templates/Proposed_Plan_2/Proposed Plan 2.xlsx
+++ b/Templates/Proposed_Plan_2/Proposed Plan 2.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\Tanmay\End Sem PBL\end-sem-practical-pbl\Templates\Proposed_Plan_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D089B3-FA56-4B37-9C95-9E67F021D84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF77562-E701-4A77-8110-4FD4FC0FB409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Student" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Student" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -239,6 +240,33 @@
   </si>
   <si>
     <t>Nikam Kabeer Atul</t>
+  </si>
+  <si>
+    <t>| 25-02-2026 | 13:30 | Both  | 2501132001 | Patil Yoksh Laxman      | 1 |</t>
+  </si>
+  <si>
+    <t>| 25-02-2026 | 13:30 | Both  | 2501132002 | Uttekar Paarth Hanumant | 1 |</t>
+  </si>
+  <si>
+    <t>| 25-02-2026 | 13:30 | Both  | 2501132003 | Gupta Aastha Vijay      | 0 |</t>
+  </si>
+  <si>
+    <t>| 25-02-2026 | 14:30 | D1    | 2501132001 | Patil Yoksh Laxman      | 1 |</t>
+  </si>
+  <si>
+    <t>| 25-02-2026 | 14:30 | D1    | 2501132002 | Uttekar Paarth Hanumant | 0 |</t>
+  </si>
+  <si>
+    <t>| 26-02-2026 | 09:30 | D2    | 2501132004 | Satvik Anand            | 1 |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRN </t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Present</t>
   </si>
 </sst>
 </file>
@@ -569,7 +597,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -635,10 +663,75 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C34F1B0-B3E1-496D-A96A-EB3225B4C563}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA5D49B-11F0-4E6C-AFFD-C0CDF29E93C5}">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="D63" sqref="D35:D63"/>
     </sheetView>
   </sheetViews>

</xml_diff>